<commit_message>
Updates to run VR tuning experiments
</commit_message>
<xml_diff>
--- a/vr_gratings_params.xlsx
+++ b/vr_gratings_params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmccann\repos\bonhoeffer\Recorder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drguggiana\PycharmProjects\Propixx_recorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>notes</t>
   </si>
@@ -50,7 +50,10 @@
     <t>[1, 5]</t>
   </si>
   <si>
-    <t>[0.00111, 0.04444]</t>
+    <t>sortby</t>
+  </si>
+  <si>
+    <t>[0.0111, 0.04444]</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -382,10 +385,11 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -402,62 +406,65 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>

</xml_diff>

<commit_message>
OSC communication for vr tuning experiments
</commit_message>
<xml_diff>
--- a/vr_gratings_params.xlsx
+++ b/vr_gratings_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>notes</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>[0.0111, 0.04444]</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>[-90, -45, 0, 45, 90]</t>
   </si>
 </sst>
 </file>
@@ -372,101 +378,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
       <c r="D2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
VR experiment base class
</commit_message>
<xml_diff>
--- a/vr_gratings_params.xlsx
+++ b/vr_gratings_params.xlsx
@@ -47,9 +47,6 @@
     <t>temporal_freq</t>
   </si>
   <si>
-    <t>[1, 5]</t>
-  </si>
-  <si>
     <t>sortby</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>[-90, -45, 0, 45, 90]</t>
+  </si>
+  <si>
+    <t>[0.5, 1, 2]</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +398,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -424,19 +424,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>

</xml_diff>

<commit_message>
Updated exerimental parameters. Added functionality for saving miniscope files in run_vr_tuning.py
</commit_message>
<xml_diff>
--- a/vr_gratings_params.xlsx
+++ b/vr_gratings_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>notes</t>
   </si>
@@ -50,16 +50,28 @@
     <t>sortby</t>
   </si>
   <si>
-    <t>[0.0111, 0.04444]</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
     <t>[-90, -45, 0, 45, 90]</t>
   </si>
   <si>
     <t>[0.5, 1, 2]</t>
+  </si>
+  <si>
+    <t>[0.02222, 0.04444]</t>
+  </si>
+  <si>
+    <t>pilot</t>
+  </si>
+  <si>
+    <t>[0.04]</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[180, 147.27, 114.54, 81.81, 49.09, 16.36, 0, -16.36, -49.09, -81.81, -114.54, -147.27]</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -424,13 +436,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -446,8 +458,27 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>

</xml_diff>